<commit_message>
add download excel button funtionality
</commit_message>
<xml_diff>
--- a/src/data/testMC.xlsx
+++ b/src/data/testMC.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\OneDrive - WageningenUR\DEVELOPMENT\mc-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E072D79A-779E-4C08-8CFA-BF2B555483B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15911C7-A759-490C-96C7-1535DAC5200D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bla" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
   <si>
     <t>team_id</t>
   </si>
@@ -289,6 +301,24 @@
   </si>
   <si>
     <t>Liver</t>
+  </si>
+  <si>
+    <t>some list</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>sadf</t>
+  </si>
+  <si>
+    <t>sda</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -304,12 +334,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -324,9 +360,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,11 +644,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH2"/>
+  <dimension ref="A1:BH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -858,117 +893,206 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45363</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44239</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44239</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>75</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A10" xr:uid="{D146312D-01E4-4944-A5DA-B597AE8EC5B0}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD8F5A6-107F-4CAB-BABF-271E80F83DDB}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>89</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>45363</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44239</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="1">
-        <v>44239</v>
-      </c>
-      <c r="G2">
-        <v>2024</v>
-      </c>
-      <c r="I2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" t="s">
-        <v>60</v>
-      </c>
-      <c r="V2" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AU2">
-        <v>75</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>81</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve reading in excel
</commit_message>
<xml_diff>
--- a/src/data/testMC.xlsx
+++ b/src/data/testMC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoend008\OneDrive - WageningenUR\DEVELOPMENT\mc-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15911C7-A759-490C-96C7-1535DAC5200D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517DB9C-BD0B-437A-BCC7-542021F85D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,7 +646,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AU1" sqref="AU1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -991,7 +993,7 @@
         <v>77</v>
       </c>
       <c r="AU2" s="1">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="AY2" s="1" t="s">
         <v>78</v>

</xml_diff>